<commit_message>
Front end & data
</commit_message>
<xml_diff>
--- a/Datos/fake_users/user1_obras.xlsx
+++ b/Datos/fake_users/user1_obras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesus\Desktop\Curso 5\Cuatri I\DAV\dav_project\datos\fake_users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50777409-C4EE-4EE6-8B8B-4A4DDA5C27DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F887DBE5-E66B-474A-9EFE-3630F955FF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Titulo</t>
   </si>
@@ -34,6 +34,76 @@
   </si>
   <si>
     <t>Valoracion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Feriantes
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Everywoman
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Misericordia
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Ricardo III
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+             Sans tambour
+            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           IRIBARNE
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Obra infinita
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Pieces of a Woman
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+            Hamlet
+           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Dragón
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Comedia sin título
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Imitation of Life
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           El patito feo
+          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+           Colgando de un hilo
+          </t>
   </si>
 </sst>
 </file>
@@ -69,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,14 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
@@ -374,6 +446,160 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45276</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45304</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45336</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45255</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45247</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45212</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44992</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44910</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44729</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44605</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44518</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44521</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45258</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>